<commit_message>
added contributions from all previsous weeks
</commit_message>
<xml_diff>
--- a/Documentation/daily-scrum-meeting.xlsx
+++ b/Documentation/daily-scrum-meeting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jclok\GitHub\MENS-SHED-SOC09109\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasti\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5791D5-23E8-4F8C-BEC0-EA47ED9530D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B65B4501-6476-43B4-B752-9ED553ED6480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18810" yWindow="1815" windowWidth="20010" windowHeight="17430" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PROJECT DETAILS" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="WK 8 06-03-23" sheetId="9" r:id="rId9"/>
     <sheet name="WK 9 13-03-23" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="124">
   <si>
     <t>DAILY SCRUM TEMPLATE</t>
   </si>
@@ -390,6 +390,30 @@
   </si>
   <si>
     <t>Mid-point report security and testing section</t>
+  </si>
+  <si>
+    <t>made my contrabutions to the PIR repot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">writing sql files for the database </t>
+  </si>
+  <si>
+    <t xml:space="preserve">looking at changes to be made for SQLite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">combined sqll files into one after forgeting upload the pervise files made for SQLite </t>
+  </si>
+  <si>
+    <t>looked in to how to displaying images in a database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the data base neededs to be rerun so no point enttering data that will be lost </t>
+  </si>
+  <si>
+    <t>made the database done, not done and risks to the mid piont report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createded files to add data into the data base </t>
   </si>
 </sst>
 </file>
@@ -689,7 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -814,6 +838,15 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="19" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -856,15 +889,6 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="19" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -900,6 +924,18 @@
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1315,18 +1351,18 @@
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,7 +1401,7 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -1376,25 +1412,25 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="48">
+      <c r="I9" s="51">
         <v>0</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="54">
         <f>SUM(I9,'WK 8 06-03-23'!J9:K11)</f>
         <v>29.6</v>
       </c>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="39" t="e">
         <f>I9/$I$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M9" s="33">
         <f>J9/$J$27</f>
-        <v>0.33277121978639684</v>
+        <v>0.29914098029307734</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1403,14 +1439,14 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="39"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -1419,14 +1455,14 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="39"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -1437,25 +1473,25 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="48">
+      <c r="I12" s="51">
         <v>0</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="54">
         <f>SUM(I12,'WK 8 06-03-23'!J12:K14)</f>
         <v>19.3</v>
       </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="39" t="e">
         <f t="shared" ref="L12:L27" si="0">I12/$I$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="33">
         <f>J12/$J$27</f>
-        <v>0.21697582911748173</v>
+        <v>0.19504800404244568</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -1464,14 +1500,14 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="39"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -1480,14 +1516,14 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="39"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -1498,25 +1534,25 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="48">
+      <c r="I15" s="51">
         <v>0</v>
       </c>
-      <c r="J15" s="51">
+      <c r="J15" s="54">
         <f>SUM(I15,'WK 8 06-03-23'!J15:K17)</f>
         <v>11.8</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="33">
         <f>J15/$J$27</f>
-        <v>0.13265879707700956</v>
+        <v>0.11925214754926731</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -1525,14 +1561,14 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="39"/>
       <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -1541,14 +1577,14 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="39"/>
       <c r="M17" s="34"/>
     </row>
     <row r="18" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -1559,25 +1595,25 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="48">
+      <c r="I18" s="51">
         <v>0</v>
       </c>
-      <c r="J18" s="51">
+      <c r="J18" s="54">
         <f>SUM(I18,'WK 8 06-03-23'!J18:K20)</f>
         <v>22.75</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="33">
         <f>J18/$J$27</f>
-        <v>0.25576166385609894</v>
+        <v>0.22991409802930773</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -1586,14 +1622,14 @@
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="39"/>
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -1602,14 +1638,14 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="39"/>
       <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -1620,25 +1656,25 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="48">
+      <c r="I21" s="51">
         <v>0</v>
       </c>
-      <c r="J21" s="51">
+      <c r="J21" s="54">
         <f>SUM(I21,'WK 8 06-03-23'!J21:K23)</f>
         <v>5.5</v>
       </c>
-      <c r="K21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M21" s="33">
         <f>J21/$J$27</f>
-        <v>6.1832490163012926E-2</v>
+        <v>5.5583628094997471E-2</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -1647,14 +1683,14 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="39"/>
       <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:13" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -1663,14 +1699,14 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="39"/>
       <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -1681,25 +1717,25 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="48">
+      <c r="I24" s="51">
         <v>0</v>
       </c>
-      <c r="J24" s="51">
+      <c r="J24" s="54">
         <f>SUM(I24,'WK 8 06-03-23'!J24:K26)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="52"/>
+        <v>10</v>
+      </c>
+      <c r="K24" s="55"/>
       <c r="L24" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M24" s="33">
         <f>J24/$J$27</f>
-        <v>0</v>
+        <v>0.10106114199090449</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
@@ -1708,14 +1744,14 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="39"/>
       <c r="M25" s="34"/>
     </row>
     <row r="26" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
@@ -1724,9 +1760,9 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="39"/>
       <c r="M26" s="34"/>
     </row>
@@ -1738,15 +1774,15 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="57">
+      <c r="I27" s="60">
         <f>SUM(I9:I26)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="57">
+      <c r="J27" s="60">
         <f>SUM(J9:K26)</f>
-        <v>88.95</v>
-      </c>
-      <c r="K27" s="59"/>
+        <v>98.95</v>
+      </c>
+      <c r="K27" s="62"/>
       <c r="L27" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1764,9 +1800,9 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
       <c r="L28" s="32"/>
       <c r="M28" s="34"/>
     </row>
@@ -1778,27 +1814,14 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
       <c r="L29" s="32"/>
       <c r="M29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:K23"/>
@@ -1807,6 +1830,19 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:K11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -1869,18 +1905,18 @@
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1921,7 +1957,7 @@
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -1942,14 +1978,14 @@
       <c r="H9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="51">
         <v>0.5</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="54">
         <f>I9</f>
         <v>0.5</v>
       </c>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="41">
         <f>I9/$I$27</f>
         <v>0.7142857142857143</v>
@@ -1960,7 +1996,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -1979,14 +2015,14 @@
       <c r="H10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="49"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="41"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -2005,14 +2041,14 @@
       <c r="H11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="41"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -2023,12 +2059,12 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="51">
+      <c r="I12" s="51"/>
+      <c r="J12" s="54">
         <f>I12</f>
         <v>0</v>
       </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="41">
         <f t="shared" ref="L12:L27" si="0">I12/$I$27</f>
         <v>0</v>
@@ -2039,7 +2075,7 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -2048,14 +2084,14 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="41"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -2064,14 +2100,14 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="41"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -2092,14 +2128,14 @@
       <c r="H15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="51">
         <v>0.2</v>
       </c>
-      <c r="J15" s="51">
+      <c r="J15" s="54">
         <f>I15</f>
         <v>0.2</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="41">
         <f t="shared" si="0"/>
         <v>0.28571428571428575</v>
@@ -2110,7 +2146,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -2129,14 +2165,14 @@
       <c r="H16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="41"/>
       <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -2155,14 +2191,14 @@
       <c r="H17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="41"/>
       <c r="M17" s="34"/>
     </row>
     <row r="18" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -2173,12 +2209,12 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="51">
+      <c r="I18" s="51"/>
+      <c r="J18" s="54">
         <f>I18</f>
         <v>0</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2189,7 +2225,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -2198,14 +2234,14 @@
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="41"/>
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -2214,14 +2250,14 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="41"/>
       <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -2232,12 +2268,12 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="51">
+      <c r="I21" s="51"/>
+      <c r="J21" s="54">
         <f>I21</f>
         <v>0</v>
       </c>
-      <c r="K21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2248,7 +2284,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -2257,14 +2293,14 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="41"/>
       <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:13" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -2273,14 +2309,14 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="41"/>
       <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -2291,12 +2327,12 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="51">
+      <c r="I24" s="51"/>
+      <c r="J24" s="54">
         <f>I24</f>
         <v>0</v>
       </c>
-      <c r="K24" s="52"/>
+      <c r="K24" s="55"/>
       <c r="L24" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2307,7 +2343,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
@@ -2316,14 +2352,14 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="41"/>
       <c r="M25" s="34"/>
     </row>
     <row r="26" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
@@ -2332,9 +2368,9 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="41"/>
       <c r="M26" s="34"/>
     </row>
@@ -2346,15 +2382,15 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="57">
+      <c r="I27" s="60">
         <f>SUM(I9:I26)</f>
         <v>0.7</v>
       </c>
-      <c r="J27" s="57">
+      <c r="J27" s="60">
         <f>SUM(J9:K26)</f>
         <v>0.7</v>
       </c>
-      <c r="K27" s="59"/>
+      <c r="K27" s="62"/>
       <c r="L27" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2372,9 +2408,9 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
       <c r="L28" s="35"/>
       <c r="M28" s="34"/>
     </row>
@@ -2386,27 +2422,14 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
       <c r="L29" s="35"/>
       <c r="M29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:K23"/>
@@ -2415,6 +2438,19 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:K11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2474,18 +2510,18 @@
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2526,7 +2562,7 @@
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -2547,14 +2583,14 @@
       <c r="H9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="51">
         <v>5.45</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="54">
         <f>SUM(I9,'WK 1 16-01-23'!J9:K11)</f>
         <v>5.95</v>
       </c>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="41">
         <f>I9/$I$27</f>
         <v>0.73154362416107388</v>
@@ -2565,7 +2601,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -2584,14 +2620,14 @@
       <c r="H10" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="49"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="41"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -2610,14 +2646,14 @@
       <c r="H11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="41"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -2628,14 +2664,14 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="48">
+      <c r="I12" s="51">
         <v>1</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="54">
         <f>SUM(I12,'WK 1 16-01-23'!J12:K14)</f>
         <v>1</v>
       </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="41">
         <f t="shared" ref="L12:L27" si="0">I12/$I$27</f>
         <v>0.13422818791946309</v>
@@ -2646,7 +2682,7 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -2657,14 +2693,14 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="41"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -2673,14 +2709,14 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="41"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -2701,14 +2737,14 @@
       <c r="H15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="51">
         <v>0.75</v>
       </c>
-      <c r="J15" s="51">
+      <c r="J15" s="54">
         <f>SUM(I15,'WK 1 16-01-23'!J15:K17)</f>
         <v>0.95</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="41">
         <f t="shared" si="0"/>
         <v>0.10067114093959731</v>
@@ -2719,7 +2755,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -2738,14 +2774,14 @@
       <c r="H16" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="41"/>
       <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -2764,14 +2800,14 @@
       <c r="H17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="41"/>
       <c r="M17" s="34"/>
     </row>
     <row r="18" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -2782,14 +2818,14 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="48">
+      <c r="I18" s="51">
         <v>0.25</v>
       </c>
-      <c r="J18" s="51">
+      <c r="J18" s="54">
         <f>SUM(I18,'WK 1 16-01-23'!J18:K20)</f>
         <v>0.25</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="41">
         <f t="shared" si="0"/>
         <v>3.3557046979865772E-2</v>
@@ -2800,7 +2836,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -2811,14 +2847,14 @@
         <v>92</v>
       </c>
       <c r="H19" s="14"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="41"/>
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -2827,14 +2863,14 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="41"/>
       <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -2845,12 +2881,12 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="51">
+      <c r="I21" s="51"/>
+      <c r="J21" s="54">
         <f>SUM(I21,'WK 1 16-01-23'!J21:K23)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2861,7 +2897,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -2870,14 +2906,14 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="41"/>
       <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:13" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -2886,14 +2922,14 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="41"/>
       <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -2904,12 +2940,12 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="51">
+      <c r="I24" s="51"/>
+      <c r="J24" s="54">
         <f>SUM(I24,'WK 1 16-01-23'!J24:K26)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="52"/>
+      <c r="K24" s="55"/>
       <c r="L24" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2920,7 +2956,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
@@ -2929,14 +2965,14 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="41"/>
       <c r="M25" s="34"/>
     </row>
     <row r="26" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
@@ -2945,9 +2981,9 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="41"/>
       <c r="M26" s="34"/>
     </row>
@@ -2959,15 +2995,15 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="57">
+      <c r="I27" s="60">
         <f>SUM(I9:I26)</f>
         <v>7.45</v>
       </c>
-      <c r="J27" s="57">
+      <c r="J27" s="60">
         <f>SUM(J9:K26)</f>
         <v>8.15</v>
       </c>
-      <c r="K27" s="59"/>
+      <c r="K27" s="62"/>
       <c r="L27" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2985,9 +3021,9 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
       <c r="L28" s="35"/>
       <c r="M28" s="34"/>
     </row>
@@ -2999,27 +3035,14 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
       <c r="L29" s="35"/>
       <c r="M29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:K23"/>
@@ -3028,6 +3051,19 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:K11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3087,18 +3123,18 @@
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3139,7 +3175,7 @@
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="2:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -3160,14 +3196,14 @@
       <c r="H9" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="51">
         <v>5.45</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="54">
         <f>SUM(I9,'WK 2 23-01-23'!J9:K11)</f>
         <v>11.4</v>
       </c>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="41">
         <f>I9/$I$27</f>
         <v>0.46382978723404256</v>
@@ -3178,7 +3214,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -3197,14 +3233,14 @@
       <c r="H10" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="49"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="41"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -3223,14 +3259,14 @@
       <c r="H11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="41"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -3245,14 +3281,14 @@
       <c r="H12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="48">
+      <c r="I12" s="51">
         <v>5</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="54">
         <f>SUM(I12,'WK 2 23-01-23'!J12:K14)</f>
         <v>6</v>
       </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="41">
         <f t="shared" ref="L12:L27" si="0">I12/$I$27</f>
         <v>0.42553191489361702</v>
@@ -3263,7 +3299,7 @@
       </c>
     </row>
     <row r="13" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -3276,14 +3312,14 @@
         <v>81</v>
       </c>
       <c r="H13" s="14"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="41"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -3292,14 +3328,14 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="41"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -3310,14 +3346,14 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="48">
+      <c r="I15" s="51">
         <v>0.3</v>
       </c>
-      <c r="J15" s="51">
+      <c r="J15" s="54">
         <f>SUM(I15,'WK 2 23-01-23'!J15:K17)</f>
         <v>1.25</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="41">
         <f t="shared" si="0"/>
         <v>2.553191489361702E-2</v>
@@ -3328,7 +3364,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -3347,14 +3383,14 @@
       <c r="H16" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="41"/>
       <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -3363,14 +3399,14 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="41"/>
       <c r="M17" s="34"/>
     </row>
     <row r="18" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -3385,14 +3421,14 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="48">
+      <c r="I18" s="51">
         <v>1</v>
       </c>
-      <c r="J18" s="51">
+      <c r="J18" s="54">
         <f>SUM(I18,'WK 2 23-01-23'!J18:K20)</f>
         <v>1.25</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="41">
         <f t="shared" si="0"/>
         <v>8.5106382978723402E-2</v>
@@ -3403,7 +3439,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -3416,14 +3452,14 @@
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="41"/>
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -3434,14 +3470,14 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="41"/>
       <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -3452,12 +3488,12 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="51">
+      <c r="I21" s="51"/>
+      <c r="J21" s="54">
         <f>SUM(I21,'WK 2 23-01-23'!J21:K23)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3468,7 +3504,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -3477,14 +3513,14 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="41"/>
       <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:13" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -3493,14 +3529,14 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="41"/>
       <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -3511,12 +3547,12 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="51">
+      <c r="I24" s="51"/>
+      <c r="J24" s="54">
         <f>SUM(I24,'WK 2 23-01-23'!J24:K26)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="52"/>
+      <c r="K24" s="55"/>
       <c r="L24" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3527,7 +3563,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
@@ -3536,14 +3572,14 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="41"/>
       <c r="M25" s="34"/>
     </row>
     <row r="26" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
@@ -3552,9 +3588,9 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="41"/>
       <c r="M26" s="34"/>
     </row>
@@ -3566,15 +3602,15 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="57">
+      <c r="I27" s="60">
         <f>SUM(I9:I26)</f>
         <v>11.75</v>
       </c>
-      <c r="J27" s="57">
+      <c r="J27" s="60">
         <f>SUM(J9:K26)</f>
         <v>19.899999999999999</v>
       </c>
-      <c r="K27" s="59"/>
+      <c r="K27" s="62"/>
       <c r="L27" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3592,9 +3628,9 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
       <c r="L28" s="35"/>
       <c r="M28" s="34"/>
     </row>
@@ -3606,27 +3642,14 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
       <c r="L29" s="35"/>
       <c r="M29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:K23"/>
@@ -3635,6 +3658,19 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:K11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3647,8 +3683,8 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="C5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,18 +3730,18 @@
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3747,7 +3783,7 @@
     </row>
     <row r="9" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -3768,26 +3804,26 @@
       <c r="H9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="51">
         <v>4.45</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="54">
         <f>SUM(I9,'WK 3 30-01-23'!J9:K11)</f>
         <v>15.850000000000001</v>
       </c>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="41">
         <f>I9/$I$27</f>
-        <v>0.23359580052493439</v>
+        <v>0.21140142517814728</v>
       </c>
       <c r="M9" s="33">
         <f>J9/$J$27</f>
-        <v>0.40693196405648269</v>
+        <v>0.38705738705738707</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -3806,15 +3842,15 @@
       <c r="H10" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="49"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="41"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -3833,15 +3869,15 @@
       <c r="H11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="41"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -3856,26 +3892,26 @@
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="48">
+      <c r="I12" s="51">
         <v>3.3</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="54">
         <f>SUM(I12,'WK 3 30-01-23'!J12:K14)</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="41">
         <f t="shared" ref="L12:L27" si="0">I12/$I$27</f>
-        <v>0.17322834645669291</v>
+        <v>0.15676959619952494</v>
       </c>
       <c r="M12" s="33">
         <f>J12/$J$27</f>
-        <v>0.23876765083440307</v>
+        <v>0.2271062271062271</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -3890,15 +3926,15 @@
         <v>63</v>
       </c>
       <c r="H13" s="14"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="41"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -3907,15 +3943,15 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="41"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -3936,26 +3972,26 @@
       <c r="H15" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="51">
         <v>4.3</v>
       </c>
-      <c r="J15" s="51">
+      <c r="J15" s="54">
         <f>SUM(I15,'WK 3 30-01-23'!J15:K17)</f>
         <v>5.55</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="41">
         <f t="shared" si="0"/>
-        <v>0.22572178477690286</v>
+        <v>0.20427553444180521</v>
       </c>
       <c r="M15" s="33">
         <f>J15/$J$27</f>
-        <v>0.14249037227214376</v>
+        <v>0.13553113553113552</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -3974,15 +4010,15 @@
       <c r="H16" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="41"/>
       <c r="M16" s="34"/>
     </row>
     <row r="17" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -4001,15 +4037,15 @@
       <c r="H17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="41"/>
       <c r="M17" s="34"/>
     </row>
     <row r="18" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -4026,26 +4062,26 @@
       <c r="H18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="48">
+      <c r="I18" s="51">
         <v>4</v>
       </c>
-      <c r="J18" s="51">
+      <c r="J18" s="54">
         <f>SUM(I18,'WK 3 30-01-23'!J18:K20)</f>
         <v>5.25</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="41">
         <f t="shared" si="0"/>
-        <v>0.20997375328083989</v>
+        <v>0.19002375296912113</v>
       </c>
       <c r="M18" s="33">
         <f>J18/$J$27</f>
-        <v>0.13478818998716302</v>
+        <v>0.12820512820512819</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -4060,15 +4096,15 @@
       <c r="H19" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="41"/>
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -4083,15 +4119,15 @@
       <c r="H20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="50"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="41"/>
       <c r="M20" s="34"/>
     </row>
     <row r="21" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -4102,26 +4138,26 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="48">
+      <c r="I21" s="51">
         <v>3</v>
       </c>
-      <c r="J21" s="51">
+      <c r="J21" s="54">
         <f>SUM(I21,'WK 3 30-01-23'!J21:K23)</f>
         <v>3</v>
       </c>
-      <c r="K21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="41">
         <f t="shared" si="0"/>
-        <v>0.15748031496062992</v>
+        <v>0.14251781472684086</v>
       </c>
       <c r="M21" s="33">
         <f>J21/$J$27</f>
-        <v>7.7021822849807436E-2</v>
+        <v>7.326007326007325E-2</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -4132,15 +4168,15 @@
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="41"/>
       <c r="M22" s="34"/>
     </row>
     <row r="23" spans="1:13" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -4149,71 +4185,75 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="41"/>
       <c r="M23" s="34"/>
     </row>
     <row r="24" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="51">
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="76">
+        <v>2</v>
+      </c>
+      <c r="J24" s="54">
         <f>SUM(I24,'WK 3 30-01-23'!J24:K26)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="52"/>
+        <v>2</v>
+      </c>
+      <c r="K24" s="55"/>
       <c r="L24" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.5011876484560567E-2</v>
       </c>
       <c r="M24" s="33">
         <f>J24/$J$27</f>
-        <v>0</v>
+        <v>4.884004884004884E-2</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="41"/>
       <c r="M25" s="34"/>
     </row>
     <row r="26" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="41"/>
       <c r="M26" s="34"/>
     </row>
@@ -4226,15 +4266,15 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="57">
+      <c r="I27" s="60">
         <f>SUM(I9:I26)</f>
-        <v>19.05</v>
-      </c>
-      <c r="J27" s="57">
+        <v>21.05</v>
+      </c>
+      <c r="J27" s="60">
         <f>SUM(J9:K26)</f>
-        <v>38.950000000000003</v>
-      </c>
-      <c r="K27" s="59"/>
+        <v>40.950000000000003</v>
+      </c>
+      <c r="K27" s="62"/>
       <c r="L27" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4253,9 +4293,9 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
       <c r="L28" s="41"/>
       <c r="M28" s="34"/>
     </row>
@@ -4268,27 +4308,14 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
       <c r="L29" s="41"/>
       <c r="M29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:K23"/>
@@ -4297,6 +4324,19 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:K11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4310,7 +4350,7 @@
   <dimension ref="B1:M29"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4358,18 +4398,18 @@
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="2:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="18"/>
     </row>
     <row r="7" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4410,7 +4450,7 @@
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -4431,25 +4471,25 @@
       <c r="H9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="51">
         <v>4.75</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="54">
         <f>SUM(I9,'WK 4 06-02-23'!J9:K11)</f>
         <v>20.6</v>
       </c>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="31">
         <f>I9/$I$27</f>
-        <v>0.2</v>
+        <v>0.19191919191919191</v>
       </c>
       <c r="M9" s="33">
         <f>J9/$J$27</f>
-        <v>0.32854864433811803</v>
+        <v>0.31354642313546421</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -4466,14 +4506,14 @@
       <c r="H10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="49"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="32"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -4492,14 +4532,14 @@
       <c r="H11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="32"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="2:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -4510,25 +4550,25 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="48">
+      <c r="I12" s="51">
         <v>4</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="54">
         <f>SUM(I12,'WK 4 06-02-23'!J12:K14)</f>
         <v>13.3</v>
       </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="31">
         <f>I12/$I$27</f>
-        <v>0.16842105263157894</v>
+        <v>0.16161616161616163</v>
       </c>
       <c r="M12" s="33">
         <f>J12/$J$27</f>
-        <v>0.21212121212121213</v>
+        <v>0.20243531202435311</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -4541,14 +4581,14 @@
       <c r="H13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="32"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -4557,14 +4597,14 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="32"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -4585,25 +4625,25 @@
       <c r="H15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="51">
         <v>6.25</v>
       </c>
-      <c r="J15" s="51">
+      <c r="J15" s="54">
         <f>SUM(I15,'WK 4 06-02-23'!J15:K17)</f>
         <v>11.8</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="31">
         <f>I15/$I$27</f>
-        <v>0.26315789473684209</v>
+        <v>0.25252525252525254</v>
       </c>
       <c r="M15" s="33">
         <f>J15/$J$27</f>
-        <v>0.18819776714513556</v>
+        <v>0.17960426179604261</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -4622,14 +4662,14 @@
       <c r="H16" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="32"/>
       <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -4648,14 +4688,14 @@
       <c r="H17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="32"/>
       <c r="M17" s="34"/>
     </row>
     <row r="18" spans="2:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -4676,25 +4716,25 @@
       <c r="H18" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="48">
+      <c r="I18" s="51">
         <v>6.25</v>
       </c>
-      <c r="J18" s="51">
+      <c r="J18" s="54">
         <f>SUM(I18,'WK 4 06-02-23'!J18:K20)</f>
         <v>11.5</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="31">
         <f>I18/$I$27</f>
-        <v>0.26315789473684209</v>
+        <v>0.25252525252525254</v>
       </c>
       <c r="M18" s="33">
         <f>J18/$J$27</f>
-        <v>0.18341307814992025</v>
+        <v>0.17503805175038051</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -4713,14 +4753,14 @@
       <c r="H19" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="32"/>
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -4739,14 +4779,14 @@
       <c r="H20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="50"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="32"/>
       <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -4757,25 +4797,25 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="48">
+      <c r="I21" s="51">
         <v>2.5</v>
       </c>
-      <c r="J21" s="51">
+      <c r="J21" s="54">
         <f>SUM(I21,'WK 4 06-02-23'!J21:K23)</f>
         <v>5.5</v>
       </c>
-      <c r="K21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="31">
         <f>I21/$I$27</f>
-        <v>0.10526315789473684</v>
+        <v>0.10101010101010101</v>
       </c>
       <c r="M21" s="33">
         <f>J21/$J$27</f>
-        <v>8.771929824561403E-2</v>
+        <v>8.3713850837138504E-2</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -4788,14 +4828,14 @@
       <c r="H22" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="32"/>
       <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -4804,14 +4844,14 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="32"/>
       <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -4822,23 +4862,25 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="51">
+      <c r="I24" s="51">
+        <v>1</v>
+      </c>
+      <c r="J24" s="54">
         <f>SUM(I24,'WK 4 06-02-23'!J24:K26)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="52"/>
+        <v>3</v>
+      </c>
+      <c r="K24" s="55"/>
       <c r="L24" s="31">
         <f>I24/$I$27</f>
-        <v>0</v>
+        <v>4.0404040404040407E-2</v>
       </c>
       <c r="M24" s="33">
         <f>J24/$J$27</f>
-        <v>0</v>
+        <v>4.5662100456621002E-2</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
@@ -4846,15 +4888,17 @@
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="H25" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I25" s="52"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="32"/>
       <c r="M25" s="34"/>
     </row>
     <row r="26" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
@@ -4863,9 +4907,9 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="32"/>
       <c r="M26" s="34"/>
     </row>
@@ -4877,15 +4921,15 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="57">
+      <c r="I27" s="60">
         <f>SUM(I9:I26)</f>
-        <v>23.75</v>
-      </c>
-      <c r="J27" s="57">
+        <v>24.75</v>
+      </c>
+      <c r="J27" s="60">
         <f>SUM(J9:K26)</f>
-        <v>62.7</v>
-      </c>
-      <c r="K27" s="59"/>
+        <v>65.7</v>
+      </c>
+      <c r="K27" s="62"/>
       <c r="L27" s="31">
         <f>I27/$I$27</f>
         <v>1</v>
@@ -4903,9 +4947,9 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
       <c r="L28" s="32"/>
       <c r="M28" s="34"/>
     </row>
@@ -4917,27 +4961,14 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
       <c r="L29" s="32"/>
       <c r="M29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:K23"/>
@@ -4946,6 +4977,19 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:K11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4959,7 +5003,7 @@
   <dimension ref="B1:M29"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5005,18 +5049,18 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="2:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="16"/>
     </row>
     <row r="7" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5057,7 +5101,7 @@
       <c r="L8" s="16"/>
     </row>
     <row r="9" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -5080,15 +5124,15 @@
       <c r="K9" s="67"/>
       <c r="L9" s="36">
         <f>I9/$I$27</f>
-        <v>0.35555555555555557</v>
+        <v>0.31372549019607843</v>
       </c>
       <c r="M9" s="37">
         <f>J9/$J$27</f>
-        <v>0.33265720081135902</v>
+        <v>0.31357552581261949</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -5110,7 +5154,7 @@
       <c r="M10" s="37"/>
     </row>
     <row r="11" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -5126,7 +5170,7 @@
       <c r="M11" s="37"/>
     </row>
     <row r="12" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -5147,15 +5191,15 @@
       <c r="K12" s="67"/>
       <c r="L12" s="36">
         <f>I12/$I$27</f>
-        <v>8.8888888888888892E-2</v>
+        <v>7.8431372549019607E-2</v>
       </c>
       <c r="M12" s="37">
         <f>J12/$J$27</f>
-        <v>0.19337390128465179</v>
+        <v>0.18228170809432759</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -5173,7 +5217,7 @@
       <c r="M13" s="37"/>
     </row>
     <row r="14" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -5189,7 +5233,7 @@
       <c r="M14" s="37"/>
     </row>
     <row r="15" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -5212,11 +5256,11 @@
       </c>
       <c r="M15" s="37">
         <f>J15/$J$27</f>
-        <v>0.15956727518593644</v>
+        <v>0.15041427660930529</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -5232,7 +5276,7 @@
       <c r="M16" s="37"/>
     </row>
     <row r="17" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -5248,7 +5292,7 @@
       <c r="M17" s="37"/>
     </row>
     <row r="18" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -5277,15 +5321,15 @@
       <c r="K18" s="67"/>
       <c r="L18" s="36">
         <f>I18/$I$27</f>
-        <v>0.55555555555555558</v>
+        <v>0.49019607843137253</v>
       </c>
       <c r="M18" s="37">
         <f>J18/$J$27</f>
-        <v>0.24002704530087896</v>
+        <v>0.22625876354365837</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -5309,7 +5353,7 @@
       <c r="M19" s="37"/>
     </row>
     <row r="20" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -5333,7 +5377,7 @@
       <c r="M20" s="37"/>
     </row>
     <row r="21" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -5356,11 +5400,11 @@
       </c>
       <c r="M21" s="37">
         <f>J21/$J$27</f>
-        <v>7.4374577417173765E-2</v>
+        <v>7.0108349267049078E-2</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -5376,7 +5420,7 @@
       <c r="M22" s="37"/>
     </row>
     <row r="23" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -5392,59 +5436,65 @@
       <c r="M23" s="37"/>
     </row>
     <row r="24" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="63"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="76">
+        <v>1.5</v>
+      </c>
       <c r="J24" s="66">
         <f>SUM(I24,'WK 5 13-02-23'!J24:K26)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="K24" s="67"/>
       <c r="L24" s="36">
         <f>I24/$I$27</f>
-        <v>0</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="M24" s="37">
         <f>J24/$J$27</f>
-        <v>0</v>
+        <v>5.736137667304015E-2</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="64"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="75" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="77"/>
       <c r="J25" s="68"/>
       <c r="K25" s="69"/>
       <c r="L25" s="36"/>
       <c r="M25" s="37"/>
     </row>
     <row r="26" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="65"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="78"/>
       <c r="J26" s="70"/>
       <c r="K26" s="71"/>
       <c r="L26" s="36"/>
@@ -5460,11 +5510,11 @@
       <c r="H27" s="15"/>
       <c r="I27" s="72">
         <f>SUM(I9:I26)</f>
-        <v>11.25</v>
+        <v>12.75</v>
       </c>
       <c r="J27" s="72">
         <f>SUM(J9:K26)</f>
-        <v>73.95</v>
+        <v>78.45</v>
       </c>
       <c r="K27" s="72"/>
       <c r="L27" s="38">
@@ -5506,19 +5556,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:K23"/>
@@ -5527,6 +5564,19 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:K11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5539,8 +5589,8 @@
   </sheetPr>
   <dimension ref="B1:M29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5587,18 +5637,18 @@
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5639,7 +5689,7 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -5650,25 +5700,25 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="48">
+      <c r="I9" s="51">
         <v>0.5</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="54">
         <f>SUM(I9,'WK 6 20-02-23 '!J9:K11)</f>
         <v>25.1</v>
       </c>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="41">
         <f>I9/$I$27</f>
-        <v>5.8823529411764705E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="M9" s="33">
         <f>J9/$J$27</f>
-        <v>0.30442692540933902</v>
+        <v>0.28060368921185019</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -5687,14 +5737,14 @@
       <c r="H10" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="I10" s="49"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="44"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -5703,14 +5753,14 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="44"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -5721,25 +5771,25 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="48">
+      <c r="I12" s="51">
         <v>3</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="54">
         <f>SUM(I12,'WK 6 20-02-23 '!J12:K14)</f>
         <v>17.3</v>
       </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="41">
         <f>I12/$I$27</f>
-        <v>0.35294117647058826</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="M12" s="33">
         <f>J12/$J$27</f>
-        <v>0.20982413583990298</v>
+        <v>0.19340413638904416</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -5752,14 +5802,14 @@
         <v>111</v>
       </c>
       <c r="H13" s="14"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="44"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -5768,14 +5818,14 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="44"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -5786,23 +5836,23 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="51">
+      <c r="I15" s="51"/>
+      <c r="J15" s="54">
         <f>SUM(I15,'WK 6 20-02-23 '!J15:K17)</f>
         <v>11.8</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="41">
         <f>I15/$I$27</f>
         <v>0</v>
       </c>
       <c r="M15" s="33">
         <f>J15/$J$27</f>
-        <v>0.14311704063068525</v>
+        <v>0.13191727221911684</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -5811,14 +5861,14 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="44"/>
       <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -5827,14 +5877,14 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="44"/>
       <c r="M17" s="34"/>
     </row>
     <row r="18" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -5851,25 +5901,25 @@
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="48">
+      <c r="I18" s="51">
         <v>5</v>
       </c>
-      <c r="J18" s="51">
+      <c r="J18" s="54">
         <f>SUM(I18,'WK 6 20-02-23 '!J18:K20)</f>
         <v>22.75</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="41">
         <f>I18/$I$27</f>
-        <v>0.58823529411764708</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="M18" s="33">
         <f>J18/$J$27</f>
-        <v>0.27592480291085503</v>
+        <v>0.25433202906651758</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -5884,14 +5934,14 @@
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="44"/>
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -5906,14 +5956,14 @@
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="44"/>
       <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -5924,23 +5974,23 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="51">
+      <c r="I21" s="51"/>
+      <c r="J21" s="54">
         <f>SUM(I21,'WK 6 20-02-23 '!J21:K23)</f>
         <v>5.5</v>
       </c>
-      <c r="K21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="41">
         <f>I21/$I$27</f>
         <v>0</v>
       </c>
       <c r="M21" s="33">
         <f>J21/$J$27</f>
-        <v>6.6707095209217707E-2</v>
+        <v>6.1486864169927331E-2</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -5949,14 +5999,14 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="44"/>
       <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:13" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -5965,14 +6015,14 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="44"/>
       <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -5983,50 +6033,56 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="51">
+      <c r="I24" s="51">
+        <v>2.5</v>
+      </c>
+      <c r="J24" s="54">
         <f>SUM(I24,'WK 6 20-02-23 '!J24:K26)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="52"/>
+        <v>7</v>
+      </c>
+      <c r="K24" s="55"/>
       <c r="L24" s="41">
         <f>I24/$I$27</f>
-        <v>0</v>
+        <v>0.22727272727272727</v>
       </c>
       <c r="M24" s="33">
         <f>J24/$J$27</f>
-        <v>0</v>
+        <v>7.825600894354387E-2</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="G25" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="H25" s="14"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="44"/>
       <c r="M25" s="34"/>
     </row>
     <row r="26" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="G26" s="14" t="s">
+        <v>121</v>
+      </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="44"/>
       <c r="M26" s="34"/>
     </row>
@@ -6038,15 +6094,15 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="57">
+      <c r="I27" s="60">
         <f>SUM(I9:I26)</f>
-        <v>8.5</v>
-      </c>
-      <c r="J27" s="57">
+        <v>11</v>
+      </c>
+      <c r="J27" s="60">
         <f>SUM(J9:K26)</f>
-        <v>82.45</v>
-      </c>
-      <c r="K27" s="59"/>
+        <v>89.45</v>
+      </c>
+      <c r="K27" s="62"/>
       <c r="L27" s="45">
         <f>SUM(L9:L26)</f>
         <v>1</v>
@@ -6064,9 +6120,9 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
       <c r="L28" s="40"/>
       <c r="M28" s="34"/>
     </row>
@@ -6078,27 +6134,14 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
       <c r="L29" s="40"/>
       <c r="M29" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:K11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="I21:I23"/>
     <mergeCell ref="J21:K23"/>
@@ -6107,6 +6150,19 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:K11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6119,8 +6175,8 @@
   </sheetPr>
   <dimension ref="B1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6155,18 +6211,18 @@
       <c r="L5" s="4"/>
     </row>
     <row r="6" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6205,7 +6261,7 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -6216,25 +6272,25 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="48">
+      <c r="I9" s="51">
         <v>4.5</v>
       </c>
-      <c r="J9" s="51">
+      <c r="J9" s="54">
         <f>SUM(I9,'WK 7 27-02-23'!J9:K11)</f>
         <v>29.6</v>
       </c>
-      <c r="K9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="41">
         <f>I9/$I$27</f>
-        <v>0.69230769230769229</v>
+        <v>0.47368421052631576</v>
       </c>
       <c r="M9" s="33">
         <f>J9/$J$27</f>
-        <v>0.33277121978639684</v>
+        <v>0.29914098029307734</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
@@ -6245,14 +6301,14 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="39"/>
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
@@ -6261,14 +6317,14 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="39"/>
       <c r="M11" s="34"/>
     </row>
     <row r="12" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -6281,25 +6337,25 @@
       <c r="H12" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="48">
+      <c r="I12" s="51">
         <v>2</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="54">
         <f>SUM(I12,'WK 7 27-02-23'!J12:K14)</f>
         <v>19.3</v>
       </c>
-      <c r="K12" s="52"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="39">
         <f t="shared" ref="L12:L27" si="0">I12/$I$27</f>
-        <v>0.30769230769230771</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="M12" s="33">
         <f>J12/$J$27</f>
-        <v>0.21697582911748173</v>
+        <v>0.19504800404244568</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
@@ -6314,14 +6370,14 @@
       <c r="H13" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="39"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
@@ -6332,14 +6388,14 @@
         <v>112</v>
       </c>
       <c r="H14" s="14"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="39"/>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -6350,23 +6406,23 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="51">
+      <c r="I15" s="51"/>
+      <c r="J15" s="54">
         <f>SUM(I15,'WK 7 27-02-23'!J15:K17)</f>
         <v>11.8</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M15" s="33">
         <f>J15/$J$27</f>
-        <v>0.13265879707700956</v>
+        <v>0.11925214754926731</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -6375,14 +6431,14 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="39"/>
       <c r="M16" s="34"/>
     </row>
     <row r="17" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -6391,14 +6447,14 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="39"/>
       <c r="M17" s="34"/>
     </row>
     <row r="18" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -6409,23 +6465,23 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="51">
+      <c r="I18" s="51"/>
+      <c r="J18" s="54">
         <f>SUM(I18,'WK 7 27-02-23'!J18:K20)</f>
         <v>22.75</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M18" s="33">
         <f>J18/$J$27</f>
-        <v>0.25576166385609894</v>
+        <v>0.22991409802930773</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
@@ -6434,14 +6490,14 @@
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="39"/>
       <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="13" t="s">
         <v>13</v>
       </c>
@@ -6450,14 +6506,14 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="39"/>
       <c r="M20" s="34"/>
     </row>
     <row r="21" spans="2:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -6468,23 +6524,23 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="51">
+      <c r="I21" s="51"/>
+      <c r="J21" s="54">
         <f>SUM(I21,'WK 7 27-02-23'!J21:K23)</f>
         <v>5.5</v>
       </c>
-      <c r="K21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M21" s="33">
         <f>J21/$J$27</f>
-        <v>6.1832490163012926E-2</v>
+        <v>5.5583628094997471E-2</v>
       </c>
     </row>
     <row r="22" spans="2:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="13" t="s">
         <v>12</v>
       </c>
@@ -6493,14 +6549,14 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="39"/>
       <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:13" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="13" t="s">
         <v>13</v>
       </c>
@@ -6509,14 +6565,14 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="39"/>
       <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -6527,39 +6583,45 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="51">
+      <c r="I24" s="51">
+        <v>3</v>
+      </c>
+      <c r="J24" s="54">
         <f>SUM(I24,'WK 7 27-02-23'!J24:K26)</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="52"/>
+        <v>10</v>
+      </c>
+      <c r="K24" s="55"/>
       <c r="L24" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.31578947368421051</v>
       </c>
       <c r="M24" s="33">
         <f>J24/$J$27</f>
-        <v>0</v>
+        <v>0.10106114199090449</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="G25" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="52"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="39"/>
       <c r="M25" s="34"/>
     </row>
     <row r="26" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="13" t="s">
         <v>13</v>
       </c>
@@ -6568,9 +6630,9 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="39"/>
       <c r="M26" s="34"/>
     </row>
@@ -6584,11 +6646,11 @@
       <c r="H27" s="15"/>
       <c r="I27" s="42">
         <f>SUM(I9:I26)</f>
-        <v>6.5</v>
-      </c>
-      <c r="J27" s="57">
+        <v>9.5</v>
+      </c>
+      <c r="J27" s="60">
         <f>SUM(J9:K26)</f>
-        <v>88.95</v>
+        <v>98.95</v>
       </c>
       <c r="K27" s="74"/>
       <c r="L27" s="39">
@@ -6630,6 +6692,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="J21:K23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="J24:K26"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:K17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="J18:K20"/>
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="I9:I11"/>
@@ -6637,19 +6712,6 @@
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="I12:I14"/>
     <mergeCell ref="J12:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:K17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="J18:K20"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="J21:K23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="J24:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>